<commit_message>
Added Constant headers to last year excel.
</commit_message>
<xml_diff>
--- a/output-excel/Secret-Santa-Game-Result-2024.xlsx
+++ b/output-excel/Secret-Santa-Game-Result-2024.xlsx
@@ -424,10 +424,10 @@
         <v>hamish.murray@acme.com</v>
       </c>
       <c r="C2" t="str">
-        <v>Mark Lawrence</v>
+        <v>Spencer Allen</v>
       </c>
       <c r="D2" t="str">
-        <v>mark.lawrence@acme.com</v>
+        <v>spencer.allen@acme.com</v>
       </c>
     </row>
     <row r="3">
@@ -438,10 +438,10 @@
         <v>layla.graham@acme.com</v>
       </c>
       <c r="C3" t="str">
-        <v>Charlie Wright</v>
+        <v>Hamish Murray</v>
       </c>
       <c r="D3" t="str">
-        <v>charlie.wright@acme.com</v>
+        <v>hamish.murray@acme.com</v>
       </c>
     </row>
     <row r="4">
@@ -455,7 +455,7 @@
         <v>Charlie Ross</v>
       </c>
       <c r="D4" t="str">
-        <v>charlie.ross@acme.com</v>
+        <v>charlie.ross.jr@acme.com</v>
       </c>
     </row>
     <row r="5">
@@ -466,10 +466,10 @@
         <v>benjamin.collins@acme.com</v>
       </c>
       <c r="C5" t="str">
-        <v>Spencer Allen</v>
+        <v>Mark Lawrence</v>
       </c>
       <c r="D5" t="str">
-        <v>spencer.allen@acme.com</v>
+        <v>mark.lawrence@acme.com</v>
       </c>
     </row>
     <row r="6">
@@ -480,10 +480,10 @@
         <v>isabella.scott@acme.com</v>
       </c>
       <c r="C6" t="str">
-        <v>Piper Stewart</v>
+        <v>Layla Graham</v>
       </c>
       <c r="D6" t="str">
-        <v>piper.stewart@acme.com</v>
+        <v>layla.graham@acme.com</v>
       </c>
     </row>
     <row r="7">
@@ -494,10 +494,10 @@
         <v>charlie.ross@acme.com</v>
       </c>
       <c r="C7" t="str">
-        <v>Benjamin Collins</v>
+        <v>Isabella Scott</v>
       </c>
       <c r="D7" t="str">
-        <v>benjamin.collins@acme.com</v>
+        <v>isabella.scott@acme.com</v>
       </c>
     </row>
     <row r="8">
@@ -511,7 +511,7 @@
         <v>Matthew King</v>
       </c>
       <c r="D8" t="str">
-        <v>matthew.king.jr@acme.com</v>
+        <v>matthew.king@acme.com</v>
       </c>
     </row>
     <row r="9">
@@ -522,10 +522,10 @@
         <v>spencer.allen@acme.com</v>
       </c>
       <c r="C9" t="str">
-        <v>Ethan Murray</v>
+        <v>Charlie Ross</v>
       </c>
       <c r="D9" t="str">
-        <v>ethan.murray@acme.com</v>
+        <v>charlie.ross@acme.com</v>
       </c>
     </row>
     <row r="10">
@@ -536,10 +536,10 @@
         <v>charlie.wright@acme.com</v>
       </c>
       <c r="C10" t="str">
-        <v>Matthew King</v>
+        <v>Piper Stewart</v>
       </c>
       <c r="D10" t="str">
-        <v>matthew.king@acme.com</v>
+        <v>piper.stewart@acme.com</v>
       </c>
     </row>
     <row r="11">
@@ -550,10 +550,10 @@
         <v>charlie.ross.jr@acme.com</v>
       </c>
       <c r="C11" t="str">
-        <v>Layla Graham</v>
+        <v>Matthew King</v>
       </c>
       <c r="D11" t="str">
-        <v>layla.graham@acme.com</v>
+        <v>matthew.king.jr@acme.com</v>
       </c>
     </row>
     <row r="12">
@@ -564,10 +564,10 @@
         <v>ethan.murray@acme.com</v>
       </c>
       <c r="C12" t="str">
-        <v>Hamish Murray</v>
+        <v>Charlie Wright</v>
       </c>
       <c r="D12" t="str">
-        <v>hamish.murray@acme.com</v>
+        <v>charlie.wright@acme.com</v>
       </c>
     </row>
     <row r="13">
@@ -578,10 +578,10 @@
         <v>matthew.king.jr@acme.com</v>
       </c>
       <c r="C13" t="str">
-        <v>Isabella Scott</v>
+        <v>Ethan Murray</v>
       </c>
       <c r="D13" t="str">
-        <v>isabella.scott@acme.com</v>
+        <v>ethan.murray@acme.com</v>
       </c>
     </row>
     <row r="14">
@@ -592,10 +592,10 @@
         <v>mark.lawrence@acme.com</v>
       </c>
       <c r="C14" t="str">
-        <v>Charlie Ross</v>
+        <v>Benjamin Collins</v>
       </c>
       <c r="D14" t="str">
-        <v>charlie.ross.jr@acme.com</v>
+        <v>benjamin.collins@acme.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>